<commit_message>
Update:  Create new HealthPredictor notebook for midterm+
* HealthPredictor.ipynb has everything we need for the midterm
* Additional changes from re-running the notebooks
</commit_message>
<xml_diff>
--- a/Data/chronickidneydisease.xlsx
+++ b/Data/chronickidneydisease.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\Projects-NB\GitHub\sockduct\HealthPredictor\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{239E8449-8FB9-4E56-8365-18FAD3F582E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F947CF9F-4D5C-40D3-95C1-E6C6FEDA6613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2850" yWindow="2250" windowWidth="27810" windowHeight="16935" xr2:uid="{883E4FEA-A8EB-4C3D-A873-068DD1666150}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{883E4FEA-A8EB-4C3D-A873-068DD1666150}"/>
   </bookViews>
   <sheets>
     <sheet name="chronickidneydisease" sheetId="1" r:id="rId1"/>
@@ -1019,7 +1019,8 @@
   <dimension ref="A1:Z401"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V8" sqref="V8"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update:  Add data READMEs, update main README+
* Main README - removed unneeded requirements
* HealthPredictor - updated some of the comments for the Exploratory
  Data Analysis pieces
* Data/README - overview of where the dataset is from
* Data/Chronic_Kidney_Disease/README - detailed overview of the original
  dataset including a reference going into further detail
</commit_message>
<xml_diff>
--- a/Data/chronickidneydisease.xlsx
+++ b/Data/chronickidneydisease.xlsx
@@ -8,22 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\Projects-NB\GitHub\sockduct\HealthPredictor\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F947CF9F-4D5C-40D3-95C1-E6C6FEDA6613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F063E006-EE3B-4BE5-B863-6CD6CF4F5CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{883E4FEA-A8EB-4C3D-A873-068DD1666150}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{883E4FEA-A8EB-4C3D-A873-068DD1666150}"/>
   </bookViews>
   <sheets>
-    <sheet name="chronickidneydisease" sheetId="1" r:id="rId1"/>
+    <sheet name="Base Dataset" sheetId="1" r:id="rId1"/>
+    <sheet name="Variables" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">chronickidneydisease!$A$1:$Z$401</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Base Dataset'!$A$1:$Z$401</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Variables!$A$1:$G$26</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4198" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4340" uniqueCount="92">
   <si>
     <t>id</t>
   </si>
@@ -156,12 +158,156 @@
   <si>
     <t>notckd</t>
   </si>
+  <si>
+    <t>Variable Name</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Demographic</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>Missing Values</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>blood pressure</t>
+  </si>
+  <si>
+    <t>mm/Hg</t>
+  </si>
+  <si>
+    <t>Categorical</t>
+  </si>
+  <si>
+    <t>specific gravity</t>
+  </si>
+  <si>
+    <t>albumin</t>
+  </si>
+  <si>
+    <t>sugar</t>
+  </si>
+  <si>
+    <t>Binary</t>
+  </si>
+  <si>
+    <t>red blood cells</t>
+  </si>
+  <si>
+    <t>pus cell</t>
+  </si>
+  <si>
+    <t>pus cell clumps</t>
+  </si>
+  <si>
+    <t>bacteria</t>
+  </si>
+  <si>
+    <t>blood glucose random</t>
+  </si>
+  <si>
+    <t>mgs/dl</t>
+  </si>
+  <si>
+    <t>blood urea</t>
+  </si>
+  <si>
+    <t>Continuous</t>
+  </si>
+  <si>
+    <t>serum creatinine</t>
+  </si>
+  <si>
+    <t>sodium</t>
+  </si>
+  <si>
+    <t>mEq/L</t>
+  </si>
+  <si>
+    <t>potassium</t>
+  </si>
+  <si>
+    <t>hemoglobin</t>
+  </si>
+  <si>
+    <t>gms</t>
+  </si>
+  <si>
+    <t>packed cell volume</t>
+  </si>
+  <si>
+    <t>wbcc</t>
+  </si>
+  <si>
+    <t>white blood cell count</t>
+  </si>
+  <si>
+    <t>cells/cmm</t>
+  </si>
+  <si>
+    <t>rbcc</t>
+  </si>
+  <si>
+    <t>red blood cell count</t>
+  </si>
+  <si>
+    <t>millions/cmm</t>
+  </si>
+  <si>
+    <t>hypertension</t>
+  </si>
+  <si>
+    <t>diabetes mellitus</t>
+  </si>
+  <si>
+    <t>coronary artery disease</t>
+  </si>
+  <si>
+    <t>appetite</t>
+  </si>
+  <si>
+    <t>pedal edema</t>
+  </si>
+  <si>
+    <t>anemia</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>ckd or not ckd</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,6 +441,19 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF303030"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF303030"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -638,9 +797,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1018,9 +1183,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66BE72A2-D073-4CFC-BB45-E89B6023431E}">
   <dimension ref="A1:Z401"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V8" sqref="V8"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30108,4 +30273,549 @@
   <autoFilter ref="A1:Z401" xr:uid="{66BE72A2-D073-4CFC-BB45-E89B6023431E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB654E0B-CBDF-4906-BBF4-FAFC324DA1BA}">
+  <dimension ref="A1:G26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:G26" xr:uid="{EB654E0B-CBDF-4906-BBF4-FAFC324DA1BA}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>